<commit_message>
file reader conectado a url_validator_app, lee el archivo y lo verifica el automata para posteriormente generar reporte en .csv
</commit_message>
<xml_diff>
--- a/documentos_prueba/test.xlsx
+++ b/documentos_prueba/test.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/ed345aa7c09ec3e8/Escritorio/UP/Septimo cuatrimestre/automatas/corte 1/automata_URLValidator/documentos_prueba/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="4" documentId="11_F25DC773A252ABDACC10481301586C405BDE58EC" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6579B10C-5BC1-4E9C-B599-86AFA4743A80}"/>
+  <xr:revisionPtr revIDLastSave="10" documentId="11_F25DC773A252ABDACC10481301586C405BDE58EC" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5B1EB8DB-B7BC-48ED-B47F-CBE8A7291B37}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -43,7 +43,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -55,6 +55,12 @@
       <u/>
       <sz val="11"/>
       <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -81,9 +87,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
@@ -100,6 +107,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -365,17 +376,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:A4"/>
+  <dimension ref="A1:A5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
+      <c r="A1" s="2">
+        <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.3">
@@ -393,12 +404,17 @@
         <v>3</v>
       </c>
     </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A1" r:id="rId1" xr:uid="{6B7242B8-2B6A-4CCA-9961-DE6E7CC50EE6}"/>
-    <hyperlink ref="A2" r:id="rId2" xr:uid="{F8A01A25-9F17-46E8-B9FD-C1C002F6AB18}"/>
-    <hyperlink ref="A3" r:id="rId3" xr:uid="{47D702A8-96C7-4433-9A3B-1F6011DF8DF4}"/>
-    <hyperlink ref="A4" r:id="rId4" xr:uid="{13891700-F82B-4A14-9F2C-D72DF5036F50}"/>
+    <hyperlink ref="A2" r:id="rId1" xr:uid="{F8A01A25-9F17-46E8-B9FD-C1C002F6AB18}"/>
+    <hyperlink ref="A3" r:id="rId2" xr:uid="{47D702A8-96C7-4433-9A3B-1F6011DF8DF4}"/>
+    <hyperlink ref="A4" r:id="rId3" xr:uid="{13891700-F82B-4A14-9F2C-D72DF5036F50}"/>
+    <hyperlink ref="A1" r:id="rId4" display="https://example.com" xr:uid="{6B7242B8-2B6A-4CCA-9961-DE6E7CC50EE6}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>